<commit_message>
#14 updated GeoSpatialDataResourceParser and data model
</commit_message>
<xml_diff>
--- a/pcor_tools/pcor_ingest/spreadsheet/GeoExposure _template.xlsx
+++ b/pcor_tools/pcor_ingest/spreadsheet/GeoExposure _template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shatzm\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pateldes/Documents/github/pcor/pcor_gen3_artifacts/pcor_tools/pcor_ingest/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C866BB33-30C6-45C7-A12E-3E923D80E438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2A4E8C-0FDA-D84E-97C3-B1264E97DEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="3570" windowWidth="25400" windowHeight="9560" xr2:uid="{BDF72E1E-7A72-4CC7-ACFD-618546E41F30}"/>
+    <workbookView xWindow="-10840" yWindow="0" windowWidth="10840" windowHeight="28800" xr2:uid="{BDF72E1E-7A72-4CC7-ACFD-618546E41F30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -726,10 +726,10 @@
     <t>use the format of region type following by specific regions</t>
   </si>
   <si>
-    <t>spatial_coverage_specific regions</t>
-  </si>
-  <si>
     <t>string, list</t>
+  </si>
+  <si>
+    <t>spatial_coverage_specific_regions</t>
   </si>
 </sst>
 </file>
@@ -875,42 +875,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -952,7 +952,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -961,19 +961,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -981,9 +978,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1304,40 +1298,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467A5F0E-AAB0-49E7-A2D8-14E53370DA7C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="35.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="26"/>
-    <col min="8" max="8" width="8.7265625" style="29"/>
-    <col min="9" max="16384" width="8.7265625" style="26"/>
+    <col min="1" max="1" width="35.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="26" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B1" s="26"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C1" s="15"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="26"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="15"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>124</v>
       </c>
@@ -1355,7 +1343,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1363,9 +1351,8 @@
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
-      <c r="H4" s="26"/>
-    </row>
-    <row r="5" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1379,9 +1366,8 @@
       <c r="E5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="26"/>
-    </row>
-    <row r="6" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1395,9 +1381,8 @@
       <c r="E6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
@@ -1411,10 +1396,9 @@
       <c r="E7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -1428,10 +1412,9 @@
       <c r="E8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1445,19 +1428,17 @@
       <c r="E9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="24"/>
       <c r="B10" s="25"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="31"/>
-      <c r="H10" s="26"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1465,10 +1446,9 @@
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="31"/>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
@@ -1483,9 +1463,8 @@
         <v>6</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="H12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
@@ -1499,10 +1478,9 @@
       <c r="E13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F13" s="31"/>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
@@ -1516,10 +1494,9 @@
       <c r="E14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
@@ -1533,10 +1510,9 @@
       <c r="E15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F15" s="32"/>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1550,28 +1526,25 @@
       <c r="E16" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="13"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
-      <c r="F17" s="32"/>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="24"/>
       <c r="B18" s="25"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="31"/>
-      <c r="H18" s="26"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
@@ -1579,10 +1552,9 @@
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="31"/>
-      <c r="H19" s="26"/>
-    </row>
-    <row r="20" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
@@ -1596,10 +1568,9 @@
       <c r="E20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="H20" s="26"/>
-    </row>
-    <row r="21" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -1613,9 +1584,8 @@
       <c r="E21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="26"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>34</v>
       </c>
@@ -1629,9 +1599,8 @@
       <c r="E22" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="26"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>36</v>
       </c>
@@ -1645,9 +1614,8 @@
       <c r="E23" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="26"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>38</v>
       </c>
@@ -1661,9 +1629,8 @@
       <c r="E24" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="26"/>
-    </row>
-    <row r="25" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
@@ -1677,9 +1644,8 @@
       <c r="E25" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="26"/>
-    </row>
-    <row r="26" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>43</v>
       </c>
@@ -1693,9 +1659,8 @@
       <c r="E26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="26"/>
-    </row>
-    <row r="27" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>46</v>
       </c>
@@ -1709,9 +1674,8 @@
       <c r="E27" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="26"/>
-    </row>
-    <row r="28" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -1725,9 +1689,8 @@
       <c r="E28" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="26"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>51</v>
       </c>
@@ -1743,9 +1706,8 @@
       <c r="E29" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H29" s="26"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>55</v>
       </c>
@@ -1761,9 +1723,8 @@
       <c r="E30" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="26"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>57</v>
       </c>
@@ -1779,9 +1740,8 @@
       <c r="E31" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="26"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>59</v>
       </c>
@@ -1795,9 +1755,8 @@
       <c r="E32" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="26"/>
-    </row>
-    <row r="33" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>61</v>
       </c>
@@ -1811,9 +1770,8 @@
       <c r="E33" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="26"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>28</v>
       </c>
@@ -1827,9 +1785,8 @@
       <c r="E34" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="26"/>
-    </row>
-    <row r="35" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>64</v>
       </c>
@@ -1843,27 +1800,23 @@
       <c r="E35" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="26"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="24"/>
-      <c r="B36" s="30"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="19"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="H36" s="26"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="26"/>
       <c r="C37" s="19"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
-      <c r="H37" s="26"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>67</v>
       </c>
@@ -1877,9 +1830,8 @@
       <c r="E38" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="26"/>
-    </row>
-    <row r="39" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>70</v>
       </c>
@@ -1893,9 +1845,8 @@
       <c r="E39" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="26"/>
-    </row>
-    <row r="40" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>72</v>
       </c>
@@ -1909,9 +1860,8 @@
       <c r="E40" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H40" s="26"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>74</v>
       </c>
@@ -1925,9 +1875,8 @@
       <c r="E41" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="26"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>76</v>
       </c>
@@ -1941,9 +1890,8 @@
       <c r="E42" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H42" s="26"/>
-    </row>
-    <row r="43" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>79</v>
       </c>
@@ -1957,9 +1905,8 @@
       <c r="E43" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="26"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>81</v>
       </c>
@@ -1973,10 +1920,9 @@
       <c r="E44" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="31"/>
-      <c r="H44" s="26"/>
-    </row>
-    <row r="45" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+      <c r="F44" s="30"/>
+    </row>
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>83</v>
       </c>
@@ -1990,19 +1936,17 @@
       <c r="E45" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F45" s="31"/>
-      <c r="H45" s="26"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F45" s="30"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="13"/>
       <c r="C46" s="19"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
-      <c r="F46" s="31"/>
-      <c r="H46" s="26"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F46" s="30"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
@@ -2010,10 +1954,9 @@
       <c r="C47" s="19"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="31"/>
-      <c r="H47" s="26"/>
-    </row>
-    <row r="48" spans="1:8" ht="124" x14ac:dyDescent="0.35">
+      <c r="F47" s="30"/>
+    </row>
+    <row r="48" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>86</v>
       </c>
@@ -2027,10 +1970,9 @@
       <c r="E48" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="31"/>
-      <c r="H48" s="26"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F48" s="30"/>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>88</v>
       </c>
@@ -2044,10 +1986,9 @@
       <c r="E49" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="31"/>
-      <c r="H49" s="26"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F49" s="30"/>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>90</v>
       </c>
@@ -2061,10 +2002,9 @@
       <c r="E50" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="31"/>
-      <c r="H50" s="26"/>
-    </row>
-    <row r="51" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>92</v>
       </c>
@@ -2078,9 +2018,8 @@
       <c r="E51" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H51" s="26"/>
-    </row>
-    <row r="52" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>94</v>
       </c>
@@ -2094,9 +2033,8 @@
       <c r="E52" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H52" s="26"/>
-    </row>
-    <row r="53" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>96</v>
       </c>
@@ -2110,9 +2048,8 @@
       <c r="E53" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H53" s="26"/>
-    </row>
-    <row r="54" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>99</v>
       </c>
@@ -2126,9 +2063,8 @@
       <c r="E54" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H54" s="26"/>
-    </row>
-    <row r="55" spans="1:8" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>102</v>
       </c>
@@ -2145,25 +2081,23 @@
       <c r="F55" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H55" s="26"/>
-    </row>
-    <row r="56" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A56" s="37" t="s">
-        <v>229</v>
+    </row>
+    <row r="56" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="35" t="s">
+        <v>230</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="21" t="s">
         <v>228</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H56" s="26"/>
-    </row>
-    <row r="57" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>105</v>
       </c>
@@ -2177,9 +2111,8 @@
       <c r="E57" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H57" s="26"/>
-    </row>
-    <row r="58" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>108</v>
       </c>
@@ -2193,9 +2126,8 @@
       <c r="E58" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H58" s="26"/>
-    </row>
-    <row r="59" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>110</v>
       </c>
@@ -2209,9 +2141,8 @@
       <c r="E59" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H59" s="26"/>
-    </row>
-    <row r="60" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>112</v>
       </c>
@@ -2225,9 +2156,8 @@
       <c r="E60" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H60" s="26"/>
-    </row>
-    <row r="61" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>114</v>
       </c>
@@ -2242,9 +2172,8 @@
         <v>9</v>
       </c>
       <c r="F61" s="10"/>
-      <c r="H61" s="26"/>
-    </row>
-    <row r="62" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>116</v>
       </c>
@@ -2258,17 +2187,15 @@
       <c r="E62" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H62" s="26"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="24"/>
       <c r="B63" s="25"/>
       <c r="C63" s="21"/>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
-      <c r="H63" s="26"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>118</v>
       </c>
@@ -2276,9 +2203,8 @@
       <c r="C64" s="19"/>
       <c r="D64" s="20"/>
       <c r="E64" s="20"/>
-      <c r="H64" s="26"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>119</v>
       </c>
@@ -2292,9 +2218,8 @@
       <c r="E65" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H65" s="26"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>121</v>
       </c>
@@ -2308,279 +2233,143 @@
       <c r="E66" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H66" s="26"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
       <c r="B67" s="13"/>
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
-      <c r="H67" s="26"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="B68" s="13"/>
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
-      <c r="H68" s="26"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B69" s="13"/>
-      <c r="H69" s="26"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B70" s="13"/>
-      <c r="H70" s="26"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B71" s="13"/>
-      <c r="H71" s="26"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B72" s="13"/>
-      <c r="H72" s="26"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B73" s="13"/>
-      <c r="H73" s="26"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B74" s="13"/>
-      <c r="H74" s="26"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B75" s="13"/>
-      <c r="H75" s="26"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B76" s="13"/>
-      <c r="H76" s="26"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B77" s="13"/>
-      <c r="H77" s="26"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B78" s="13"/>
-      <c r="H78" s="26"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B79" s="13"/>
-      <c r="H79" s="26"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B80" s="13"/>
-      <c r="H80" s="26"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" s="13"/>
-      <c r="H81" s="26"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B82" s="26"/>
-      <c r="H82" s="26"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B83" s="26"/>
-      <c r="H83" s="26"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" s="13"/>
-      <c r="H84" s="26"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" s="13"/>
-      <c r="H85" s="26"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" s="13"/>
-      <c r="H86" s="26"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" s="13"/>
-      <c r="H87" s="26"/>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" s="13"/>
-      <c r="H88" s="26"/>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" s="13"/>
-      <c r="H89" s="26"/>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" s="13"/>
-      <c r="H90" s="26"/>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" s="13"/>
-      <c r="H91" s="26"/>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" s="13"/>
-      <c r="H92" s="26"/>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" s="13"/>
-      <c r="H93" s="26"/>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" s="13"/>
-      <c r="H94" s="26"/>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" s="13"/>
-      <c r="H95" s="26"/>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" s="13"/>
-      <c r="H96" s="26"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" s="13"/>
-      <c r="H97" s="26"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" s="13"/>
-      <c r="H98" s="26"/>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" s="13"/>
-      <c r="H99" s="26"/>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" s="13"/>
-      <c r="H100" s="26"/>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" s="13"/>
-      <c r="H101" s="26"/>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" s="13"/>
-      <c r="H102" s="26"/>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" s="13"/>
-      <c r="H103" s="26"/>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" s="13"/>
-      <c r="H104" s="26"/>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" s="13"/>
-      <c r="H105" s="26"/>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" s="13"/>
-      <c r="H106" s="26"/>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" s="13"/>
-      <c r="H107" s="26"/>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" s="13"/>
-      <c r="H108" s="26"/>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" s="13"/>
-      <c r="H109" s="26"/>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" s="13"/>
-      <c r="H110" s="26"/>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" s="13"/>
-      <c r="H111" s="26"/>
-    </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B112" s="26"/>
-      <c r="H112" s="26"/>
-    </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B113" s="26"/>
-      <c r="H113" s="26"/>
-    </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B114" s="26"/>
-      <c r="H114" s="26"/>
-    </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B115" s="26"/>
-      <c r="H115" s="26"/>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B116" s="26"/>
-      <c r="H116" s="26"/>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B117" s="26"/>
-      <c r="H117" s="26"/>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B118" s="26"/>
-      <c r="H118" s="26"/>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B119" s="26"/>
-      <c r="H119" s="26"/>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B120" s="26"/>
-      <c r="H120" s="26"/>
-    </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B121" s="26"/>
-      <c r="H121" s="26"/>
-    </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B122" s="26"/>
-      <c r="H122" s="26"/>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B123" s="26"/>
-      <c r="H123" s="26"/>
-    </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B124" s="26"/>
-      <c r="H124" s="26"/>
-    </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B125" s="26"/>
-      <c r="H125" s="26"/>
-    </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B126" s="26"/>
-      <c r="H126" s="26"/>
-    </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B127" s="26"/>
-      <c r="H127" s="26"/>
-    </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B128" s="26"/>
-      <c r="H128" s="26"/>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B129" s="26"/>
-      <c r="H129" s="26"/>
-    </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B130" s="26"/>
-      <c r="H130" s="26"/>
-    </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B131" s="26"/>
-      <c r="H131" s="26"/>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B132" s="26"/>
-      <c r="H132" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2729,105 +2518,105 @@
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" style="2"/>
-    <col min="3" max="3" width="23" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" style="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="47.6328125" style="35" customWidth="1"/>
-    <col min="15" max="15" width="22.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.54296875" style="35" customWidth="1"/>
-    <col min="18" max="18" width="15.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.08984375" style="35" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.08984375" style="35" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="15.81640625" style="35"/>
+    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="2"/>
+    <col min="3" max="3" width="23" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.6640625" style="34" customWidth="1"/>
+    <col min="15" max="15" width="22.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5" style="34" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.1640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="15.83203125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="34" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="33" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>46</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="W1" s="30" t="s">
         <v>119</v>
       </c>
       <c r="X1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -2879,7 +2668,7 @@
       <c r="R2" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="S2" s="2" t="s">
         <v>188</v>
       </c>
       <c r="T2" s="2" t="s">
@@ -2898,321 +2687,321 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="P3" s="35" t="s">
+      <c r="P3" s="34" t="s">
         <v>179</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="R3" s="35" t="s">
+      <c r="R3" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="S3" s="35" t="s">
+      <c r="S3" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="T3" s="35" t="s">
+      <c r="T3" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="U3" s="35" t="s">
+      <c r="U3" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="V3" s="35" t="s">
+      <c r="V3" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="W3" s="35" t="s">
+      <c r="W3" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="X3" s="35" t="s">
+      <c r="X3" s="34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="C4" s="35" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C4" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="O4" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="Q4" s="35" t="s">
+      <c r="Q4" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="R4" s="35" t="s">
+      <c r="R4" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="T4" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="U4" s="35" t="s">
+      <c r="U4" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="V4" s="35" t="s">
+      <c r="V4" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="W4" s="35" t="s">
+      <c r="W4" s="34" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="C5" s="35" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="C5" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="R5" s="35" t="s">
+      <c r="R5" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="T5" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="V5" s="35" t="s">
+      <c r="V5" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="W5" s="35" t="s">
+      <c r="W5" s="34" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F6" s="35" t="s">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F6" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="Q6" s="35" t="s">
+      <c r="Q6" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="T6" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="V6" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="W6" s="35" t="s">
+      <c r="W6" s="34" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F7" s="35" t="s">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F7" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="Q7" s="35" t="s">
+      <c r="Q7" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="T7" s="35" t="s">
+      <c r="T7" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="V7" s="35" t="s">
+      <c r="V7" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="W7" s="35" t="s">
+      <c r="W7" s="34" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F8" s="35" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F8" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="Q8" s="35" t="s">
+      <c r="Q8" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="T8" s="35" t="s">
+      <c r="T8" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="V8" s="35" t="s">
+      <c r="V8" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="W8" s="35" t="s">
+      <c r="W8" s="34" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F9" s="35" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F9" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="Q9" s="35" t="s">
+      <c r="Q9" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="T9" s="35" t="s">
+      <c r="T9" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="V9" s="35" t="s">
+      <c r="V9" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="W9" s="34" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F10" s="35" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F10" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="T10" s="35" t="s">
+      <c r="T10" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="V10" s="35" t="s">
+      <c r="V10" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="W10" s="35" t="s">
+      <c r="W10" s="34" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F11" s="35" t="s">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F11" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="Q11" s="35" t="s">
+      <c r="Q11" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="T11" s="35" t="s">
+      <c r="T11" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="V11" s="35" t="s">
+      <c r="V11" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="W11" s="35" t="s">
+      <c r="W11" s="34" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F12" s="35" t="s">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F12" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="T12" s="35" t="s">
+      <c r="T12" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="V12" s="35" t="s">
+      <c r="V12" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="W12" s="35" t="s">
+      <c r="W12" s="34" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F13" s="35" t="s">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F13" s="34" t="s">
         <v>170</v>
       </c>
       <c r="K13" s="6"/>
-      <c r="V13" s="35" t="s">
+      <c r="V13" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="W13" s="35" t="s">
+      <c r="W13" s="34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F14" s="35" t="s">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F14" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="V14" s="35" t="s">
+      <c r="V14" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="W14" s="35" t="s">
+      <c r="W14" s="34" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="F15" s="35" t="s">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F15" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="V15" s="35" t="s">
+      <c r="V15" s="34" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="R16" s="10"/>
-      <c r="V16" s="35" t="s">
+      <c r="V16" s="34" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
   </sheetData>

</xml_diff>